<commit_message>
Added Gitbook Docs; updated test.html
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaypung/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaypung/work/pathdao/sendnft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B058C290-EAD5-0D43-A48A-FA384AB081F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E99C1C-E4C9-A549-B830-25348063E8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14600" yWindow="23780" windowWidth="28040" windowHeight="17440" xr2:uid="{10A82438-B024-8842-A9FF-F2C9000580FE}"/>
+    <workbookView xWindow="-34160" yWindow="1000" windowWidth="28040" windowHeight="17440" xr2:uid="{10A82438-B024-8842-A9FF-F2C9000580FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Wallet Address</t>
   </si>
@@ -44,35 +44,26 @@
     <t>Token Id</t>
   </si>
   <si>
-    <t>0x38d3B085D181e4ceb0af496C6E065d518163ae93</t>
-  </si>
-  <si>
-    <t>0x037571C1115E06A2Fb9e57B3D14Ab53B5D7132b1</t>
+    <t>0x8321c738ed49310bb600fa2631651db4aa411676</t>
+  </si>
+  <si>
+    <t>0x440efbDd6c2654E7A8062afcd7754C5E8C6f74AD</t>
+  </si>
+  <si>
+    <t>0x319711283DA738C42C50ec0C7675626dFaccEc63</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF24272A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FFE8E6E3"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,10 +86,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,11 +404,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FD21AF-51F1-644A-8958-227F4C4E7BAF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="43.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -432,30 +424,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>